<commit_message>
Fixed medication export issue AB#12255
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/MedicationReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/MedicationReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F579F505-E8BF-7E46-99D8-52AED3F4903C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646CA638-967C-4DAF-9B5E-2A0359CAED47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +109,12 @@
   </si>
   <si>
     <t>{d.records[i+1].manufacturer}</t>
+  </si>
+  <si>
+    <t>{d.records[i].brand}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].brand}</t>
   </si>
 </sst>
 </file>
@@ -485,18 +490,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="3" max="5" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.296875" customWidth="1"/>
+    <col min="3" max="5" width="35.796875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" customWidth="1"/>
-    <col min="9" max="9" width="44.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.796875" customWidth="1"/>
+    <col min="9" max="9" width="44.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -533,7 +540,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -554,7 +561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -562,7 +569,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Fixed medication export issue AB#12255 (#3251)
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/MedicationReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/MedicationReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F579F505-E8BF-7E46-99D8-52AED3F4903C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646CA638-967C-4DAF-9B5E-2A0359CAED47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +109,12 @@
   </si>
   <si>
     <t>{d.records[i+1].manufacturer}</t>
+  </si>
+  <si>
+    <t>{d.records[i].brand}</t>
+  </si>
+  <si>
+    <t>{d.records[i+1].brand}</t>
   </si>
 </sst>
 </file>
@@ -485,18 +490,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="3" max="5" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.296875" customWidth="1"/>
+    <col min="3" max="5" width="35.796875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" customWidth="1"/>
-    <col min="9" max="9" width="44.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.796875" customWidth="1"/>
+    <col min="9" max="9" width="44.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -533,7 +540,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -554,7 +561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -562,7 +569,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>

</xml_diff>